<commit_message>
Added negatives and finished assignment 2.
</commit_message>
<xml_diff>
--- a/Avg runtime.xlsx
+++ b/Avg runtime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom_s\Desktop\HPP\github\HPP_bucketsort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A088FE3-7E0C-468C-9AE8-D7A6BC0DDA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242770EC-4119-4E07-B20D-5E4B8303D10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="19230" windowWidth="16410" windowHeight="8955" xr2:uid="{4A86331E-29B7-44E7-A10F-EE6EFBE688F0}"/>
+    <workbookView xWindow="120" yWindow="19395" windowWidth="16410" windowHeight="8865" xr2:uid="{4A86331E-29B7-44E7-A10F-EE6EFBE688F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -399,12 +399,12 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -424,12 +424,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -446,7 +446,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>100</v>
       </c>
@@ -454,7 +454,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1000</v>
       </c>
@@ -462,7 +462,7 @@
         <v>0.10199999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10000</v>
       </c>

</xml_diff>

<commit_message>
Update Parallel Merge Sort - code and report (unfinished).
</commit_message>
<xml_diff>
--- a/Avg runtime.xlsx
+++ b/Avg runtime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom_s\Desktop\HPP\github\HPP_bucketsort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242770EC-4119-4E07-B20D-5E4B8303D10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882F1E35-D073-4B3C-92E2-E6C94B1C43CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="19395" windowWidth="16410" windowHeight="8865" xr2:uid="{4A86331E-29B7-44E7-A10F-EE6EFBE688F0}"/>
+    <workbookView xWindow="-19310" yWindow="810" windowWidth="19420" windowHeight="10300" xr2:uid="{4A86331E-29B7-44E7-A10F-EE6EFBE688F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>n</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t>runs: 1000</t>
+  </si>
+  <si>
+    <t>Bucket sort</t>
+  </si>
+  <si>
+    <t>Parellel merge</t>
+  </si>
+  <si>
+    <t>runtime</t>
   </si>
 </sst>
 </file>
@@ -396,78 +405,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73143D92-8E27-4BB6-85B2-44A4B610A706}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
+      <c r="C1">
         <v>10</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>100</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>1000</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>10000</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3">
         <v>10</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>1.4E-2</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4">
         <v>100</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5">
         <v>1000</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>0.10199999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>10000</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.80800000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update parallel merge - limit.
</commit_message>
<xml_diff>
--- a/Avg runtime.xlsx
+++ b/Avg runtime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom_s\Desktop\HPP\github\HPP_bucketsort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882F1E35-D073-4B3C-92E2-E6C94B1C43CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C6DEA5-7023-4533-97C8-57F15D063545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="810" windowWidth="19420" windowHeight="10300" xr2:uid="{4A86331E-29B7-44E7-A10F-EE6EFBE688F0}"/>
+    <workbookView xWindow="2400" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{4A86331E-29B7-44E7-A10F-EE6EFBE688F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
     <t>Parellel merge</t>
   </si>
   <si>
-    <t>runtime</t>
+    <t>threads</t>
   </si>
 </sst>
 </file>
@@ -405,18 +405,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73143D92-8E27-4BB6-85B2-44A4B610A706}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -439,12 +439,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>10</v>
       </c>
@@ -461,7 +461,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>100</v>
       </c>
@@ -469,7 +469,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1000</v>
       </c>
@@ -477,7 +477,7 @@
         <v>0.10199999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>10000</v>
       </c>
@@ -485,37 +485,51 @@
         <v>0.80800000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
         <v>5</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>8</v>
       </c>
       <c r="H8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12">
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13">
         <v>10000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update parrellel merge - amount of threads.
</commit_message>
<xml_diff>
--- a/Avg runtime.xlsx
+++ b/Avg runtime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom_s\Desktop\HPP\github\HPP_bucketsort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C6DEA5-7023-4533-97C8-57F15D063545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA786DD-2981-4FD5-9D1A-B66F0ABF03D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{4A86331E-29B7-44E7-A10F-EE6EFBE688F0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4A86331E-29B7-44E7-A10F-EE6EFBE688F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>n</t>
   </si>
@@ -54,12 +54,66 @@
   </si>
   <si>
     <t>threads</t>
+  </si>
+  <si>
+    <t>0.000192</t>
+  </si>
+  <si>
+    <t>0.000426</t>
+  </si>
+  <si>
+    <t>0.000763</t>
+  </si>
+  <si>
+    <t>0.00108</t>
+  </si>
+  <si>
+    <t>0.00061</t>
+  </si>
+  <si>
+    <t>0.000607</t>
+  </si>
+  <si>
+    <t>0.000800</t>
+  </si>
+  <si>
+    <t>0.00133</t>
+  </si>
+  <si>
+    <t>0.00349</t>
+  </si>
+  <si>
+    <t>0.00289</t>
+  </si>
+  <si>
+    <t>0.00243</t>
+  </si>
+  <si>
+    <t>0.00196</t>
+  </si>
+  <si>
+    <t>0.02699</t>
+  </si>
+  <si>
+    <t>0.0171</t>
+  </si>
+  <si>
+    <t>0.01313</t>
+  </si>
+  <si>
+    <t>0.01166</t>
+  </si>
+  <si>
+    <t>runs: 100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,8 +143,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -405,15 +460,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73143D92-8E27-4BB6-85B2-44A4B610A706}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="3" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -505,7 +561,7 @@
         <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -522,18 +578,72 @@
       <c r="B11">
         <v>100</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>1000</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>10000</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>100000</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Array Sum - working parrallel arraysum with omp.
</commit_message>
<xml_diff>
--- a/Avg runtime.xlsx
+++ b/Avg runtime.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom_s\Desktop\HPP\github\HPP_bucketsort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA786DD-2981-4FD5-9D1A-B66F0ABF03D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8363A3A1-AEB9-4F3A-99DE-1DBABAD62EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4A86331E-29B7-44E7-A10F-EE6EFBE688F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4A86331E-29B7-44E7-A10F-EE6EFBE688F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>n</t>
   </si>
@@ -105,6 +105,24 @@
   </si>
   <si>
     <t>runs: 100</t>
+  </si>
+  <si>
+    <t>t(sec)</t>
+  </si>
+  <si>
+    <t>1 thread</t>
+  </si>
+  <si>
+    <t>2 thread</t>
+  </si>
+  <si>
+    <t>4 thread</t>
+  </si>
+  <si>
+    <t>8 thread</t>
+  </si>
+  <si>
+    <t>t((sec)</t>
   </si>
 </sst>
 </file>
@@ -112,12 +130,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -139,13 +163,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -460,19 +501,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73143D92-8E27-4BB6-85B2-44A4B610A706}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="3" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+    <col min="3" max="6" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -495,12 +536,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>10</v>
       </c>
@@ -517,7 +558,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>100</v>
       </c>
@@ -525,7 +566,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>1000</v>
       </c>
@@ -533,7 +574,7 @@
         <v>0.10199999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>10000</v>
       </c>
@@ -541,7 +582,7 @@
         <v>0.80800000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -564,17 +605,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>100</v>
       </c>
@@ -591,7 +632,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>1000</v>
       </c>
@@ -608,7 +649,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>10000</v>
       </c>
@@ -625,7 +666,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>100000</v>
       </c>
@@ -642,7 +683,202 @@
         <v>21</v>
       </c>
     </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>10000</v>
+      </c>
+      <c r="C17">
+        <v>2.7E-2</v>
+      </c>
+      <c r="D17">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E17">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F17">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G17">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <v>100000</v>
+      </c>
+      <c r="C18">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="D18">
+        <v>1.6E-2</v>
+      </c>
+      <c r="E18">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F18">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G18">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>1000000</v>
+      </c>
+      <c r="C19">
+        <v>2.4969999999999999</v>
+      </c>
+      <c r="D19">
+        <v>0.124</v>
+      </c>
+      <c r="E19">
+        <v>0.124</v>
+      </c>
+      <c r="F19">
+        <v>0.124</v>
+      </c>
+      <c r="G19">
+        <v>0.124</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <v>10000000</v>
+      </c>
+      <c r="C20">
+        <v>24.792999999999999</v>
+      </c>
+      <c r="D20">
+        <v>1.2170000000000001</v>
+      </c>
+      <c r="E20">
+        <v>1.2090000000000001</v>
+      </c>
+      <c r="F20">
+        <v>1.206</v>
+      </c>
+      <c r="G20">
+        <v>1.204</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C24" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D24" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E24" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F24" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B25" s="2">
+        <v>100000</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1.4E-2</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B26" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.124</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.124</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.124</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.124</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B27" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1.2170000000000001</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1.2090000000000001</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1.206</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1.204</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
4. CSP - fixed multithreading with unsighed variables.
</commit_message>
<xml_diff>
--- a/Avg runtime.xlsx
+++ b/Avg runtime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom_s\Desktop\HPP\github\HPP_bucketsort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8363A3A1-AEB9-4F3A-99DE-1DBABAD62EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8A5F51-5C79-4B65-8AF8-6ED49A9E12C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4A86331E-29B7-44E7-A10F-EE6EFBE688F0}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11235" xr2:uid="{4A86331E-29B7-44E7-A10F-EE6EFBE688F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>n</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>t((sec)</t>
+  </si>
+  <si>
+    <t>circuit satisfiability problem</t>
+  </si>
+  <si>
+    <t>cores</t>
+  </si>
+  <si>
+    <t>runtime (micro seconds)</t>
   </si>
 </sst>
 </file>
@@ -132,7 +141,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +151,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -182,11 +199,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -202,6 +220,1005 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$B$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cores</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Blad1!$B$31:$B$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$B$31:$B$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A0D4-4430-90A0-DFF2A76E8F2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$C$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>runtime (micro seconds)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Blad1!$B$31:$B$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$C$31:$C$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="0.00000">
+                  <c:v>381483408</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>209677767</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>108613141</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60065594</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A0D4-4430-90A0-DFF2A76E8F2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1127630544"/>
+        <c:axId val="1186192464"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1127630544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1186192464"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1186192464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1127630544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>363140</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>170259</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>77390</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>55959</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafiek 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C93F7985-6901-D460-8C5B-01F941DFCEDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -501,19 +1518,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73143D92-8E27-4BB6-85B2-44A4B610A706}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" customWidth="1"/>
-    <col min="3" max="6" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -536,12 +1554,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>10</v>
       </c>
@@ -558,7 +1576,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>100</v>
       </c>
@@ -566,7 +1584,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1000</v>
       </c>
@@ -574,7 +1592,7 @@
         <v>0.10199999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>10000</v>
       </c>
@@ -582,7 +1600,7 @@
         <v>0.80800000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -605,17 +1623,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>100</v>
       </c>
@@ -632,7 +1650,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>1000</v>
       </c>
@@ -649,7 +1667,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10000</v>
       </c>
@@ -666,7 +1684,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>100000</v>
       </c>
@@ -683,7 +1701,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>0</v>
       </c>
@@ -703,7 +1721,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>10000</v>
       </c>
@@ -723,7 +1741,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>100000</v>
       </c>
@@ -743,7 +1761,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>1000000</v>
       </c>
@@ -763,7 +1781,7 @@
         <v>0.124</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>10000000</v>
       </c>
@@ -783,7 +1801,7 @@
         <v>1.204</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
         <v>28</v>
@@ -792,7 +1810,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>0</v>
       </c>
@@ -809,7 +1827,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>10000</v>
       </c>
@@ -826,7 +1844,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>100000</v>
       </c>
@@ -843,7 +1861,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>1000000</v>
       </c>
@@ -860,7 +1878,7 @@
         <v>0.124</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>10000000</v>
       </c>
@@ -875,11 +1893,57 @@
       </c>
       <c r="F27" s="2">
         <v>1.204</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>381483408</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <v>2</v>
+      </c>
+      <c r="C32" s="2">
+        <v>209677767</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <v>4</v>
+      </c>
+      <c r="C33" s="2">
+        <v>108613141</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <v>8</v>
+      </c>
+      <c r="C34" s="2">
+        <v>60065594</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Zeef - last update: working with mpi and omp.
</commit_message>
<xml_diff>
--- a/Avg runtime.xlsx
+++ b/Avg runtime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom_s\Desktop\HPP\github\HPP_bucketsort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8A5F51-5C79-4B65-8AF8-6ED49A9E12C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50954CB-EA4A-40FD-B471-F298CA30C922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11235" xr2:uid="{4A86331E-29B7-44E7-A10F-EE6EFBE688F0}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4A86331E-29B7-44E7-A10F-EE6EFBE688F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>n</t>
   </si>
@@ -132,6 +132,15 @@
   </si>
   <si>
     <t>runtime (micro seconds)</t>
+  </si>
+  <si>
+    <t>zeef</t>
+  </si>
+  <si>
+    <t>threads &amp; processors</t>
+  </si>
+  <si>
+    <t>runtime</t>
   </si>
 </sst>
 </file>
@@ -1518,10 +1527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73143D92-8E27-4BB6-85B2-44A4B610A706}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1940,6 +1949,42 @@
         <v>60065594</v>
       </c>
     </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>